<commit_message>
Changed the JSON to correct some errors in the data
</commit_message>
<xml_diff>
--- a/madmen/madmendata.xlsx
+++ b/madmen/madmendata.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0badd7e539d441f0/Documents/Codes/Codes November/madmen/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="98">
   <si>
     <t>Episode</t>
   </si>
@@ -309,13 +305,22 @@
   </si>
   <si>
     <t>Episode Number</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Users</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -395,6 +400,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -457,7 +474,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -492,7 +509,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -669,28 +686,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="5" customWidth="1"/>
     <col min="3" max="4" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -704,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -718,7 +733,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="60" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -732,7 +747,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" customHeight="1">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -746,7 +761,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="45" customHeight="1">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -760,7 +775,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45" customHeight="1">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -774,7 +789,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" customHeight="1">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -788,7 +803,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="45" customHeight="1">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -802,7 +817,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="75" customHeight="1">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -816,7 +831,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -830,7 +845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="45" customHeight="1">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -844,7 +859,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="45" customHeight="1">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -858,7 +873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="45" customHeight="1">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -872,7 +887,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="45" customHeight="1">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -886,7 +901,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="45" customHeight="1">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -900,7 +915,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -914,7 +929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="30" customHeight="1">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -928,7 +943,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="30" customHeight="1">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -942,7 +957,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="60" customHeight="1">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -956,7 +971,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="45" customHeight="1">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -970,7 +985,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="30" customHeight="1">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -984,7 +999,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="60" customHeight="1">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -998,7 +1013,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="45" customHeight="1">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -1012,7 +1027,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="45" customHeight="1">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1026,7 +1041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="45" customHeight="1">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -1040,7 +1055,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30" customHeight="1">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -1054,7 +1069,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="90" customHeight="1">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -1068,7 +1083,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="30" customHeight="1">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -1082,7 +1097,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="30" customHeight="1">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -1096,7 +1111,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="45" customHeight="1">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -1110,7 +1125,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="60" customHeight="1">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -1124,7 +1139,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="45" customHeight="1">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -1138,7 +1153,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="30" customHeight="1">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -1152,7 +1167,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="45" customHeight="1">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -1166,7 +1181,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="30" customHeight="1">
       <c r="A35" s="1">
         <v>3</v>
       </c>
@@ -1180,7 +1195,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="45" customHeight="1">
       <c r="A36" s="1">
         <v>3</v>
       </c>
@@ -1194,7 +1209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="30" customHeight="1">
       <c r="A37" s="1">
         <v>3</v>
       </c>
@@ -1208,7 +1223,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="60" customHeight="1">
       <c r="A38" s="1">
         <v>3</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="45" customHeight="1">
       <c r="A39" s="1">
         <v>3</v>
       </c>
@@ -1236,7 +1251,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="45" customHeight="1">
       <c r="A40" s="1">
         <v>4</v>
       </c>
@@ -1250,7 +1265,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="30" customHeight="1">
       <c r="A41" s="1">
         <v>4</v>
       </c>
@@ -1264,7 +1279,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="30" customHeight="1">
       <c r="A42" s="1">
         <v>4</v>
       </c>
@@ -1278,7 +1293,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="45" customHeight="1">
       <c r="A43" s="1">
         <v>4</v>
       </c>
@@ -1292,7 +1307,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="30" customHeight="1">
       <c r="A44" s="1">
         <v>4</v>
       </c>
@@ -1306,7 +1321,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="30" customHeight="1">
       <c r="A45" s="1">
         <v>4</v>
       </c>
@@ -1320,7 +1335,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="30">
       <c r="A46" s="1">
         <v>4</v>
       </c>
@@ -1334,7 +1349,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="60" customHeight="1">
       <c r="A47" s="1">
         <v>4</v>
       </c>
@@ -1348,7 +1363,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="30" customHeight="1">
       <c r="A48" s="1">
         <v>4</v>
       </c>
@@ -1362,7 +1377,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="30" customHeight="1">
       <c r="A49" s="1">
         <v>4</v>
       </c>
@@ -1376,7 +1391,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="45" customHeight="1">
       <c r="A50" s="1">
         <v>4</v>
       </c>
@@ -1390,7 +1405,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="30" customHeight="1">
       <c r="A51" s="1">
         <v>4</v>
       </c>
@@ -1404,7 +1419,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="45" customHeight="1">
       <c r="A52" s="1">
         <v>4</v>
       </c>
@@ -1418,7 +1433,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="45" customHeight="1">
       <c r="A53" s="1">
         <v>5</v>
       </c>
@@ -1432,7 +1447,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="30" customHeight="1">
       <c r="A54" s="1">
         <v>5</v>
       </c>
@@ -1446,7 +1461,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="45" customHeight="1">
       <c r="A55" s="1">
         <v>5</v>
       </c>
@@ -1460,7 +1475,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="45" customHeight="1">
       <c r="A56" s="1">
         <v>5</v>
       </c>
@@ -1474,7 +1489,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="30" customHeight="1">
       <c r="A57" s="1">
         <v>5</v>
       </c>
@@ -1488,7 +1503,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="45" customHeight="1">
       <c r="A58" s="1">
         <v>5</v>
       </c>
@@ -1502,7 +1517,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="30" customHeight="1">
       <c r="A59" s="1">
         <v>5</v>
       </c>
@@ -1516,7 +1531,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="30" customHeight="1">
       <c r="A60" s="1">
         <v>5</v>
       </c>
@@ -1530,7 +1545,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="1">
         <v>5</v>
       </c>
@@ -1544,7 +1559,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="1">
         <v>5</v>
       </c>
@@ -1558,7 +1573,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="1">
         <v>5</v>
       </c>
@@ -1572,7 +1587,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="45" customHeight="1">
       <c r="A64" s="1">
         <v>5</v>
       </c>
@@ -1586,7 +1601,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="30" customHeight="1">
       <c r="A65" s="1">
         <v>5</v>
       </c>
@@ -1600,7 +1615,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="30" customHeight="1">
       <c r="A66" s="1">
         <v>6</v>
       </c>
@@ -1614,7 +1629,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="30" customHeight="1">
       <c r="A67" s="1">
         <v>6</v>
       </c>
@@ -1628,7 +1643,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="60" customHeight="1">
       <c r="A68" s="1">
         <v>6</v>
       </c>
@@ -1642,7 +1657,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="60" customHeight="1">
       <c r="A69" s="1">
         <v>6</v>
       </c>
@@ -1656,7 +1671,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="45" customHeight="1">
       <c r="A70" s="1">
         <v>6</v>
       </c>
@@ -1670,7 +1685,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="1">
         <v>6</v>
       </c>
@@ -1684,7 +1699,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="30" customHeight="1">
       <c r="A72" s="1">
         <v>6</v>
       </c>
@@ -1698,7 +1713,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="45" customHeight="1">
       <c r="A73" s="1">
         <v>6</v>
       </c>
@@ -1712,7 +1727,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="1">
         <v>6</v>
       </c>
@@ -1726,7 +1741,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="45" customHeight="1">
       <c r="A75" s="1">
         <v>6</v>
       </c>
@@ -1740,7 +1755,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="75" customHeight="1">
       <c r="A76" s="1">
         <v>6</v>
       </c>
@@ -1754,7 +1769,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="45" customHeight="1">
       <c r="A77" s="1">
         <v>6</v>
       </c>
@@ -1768,7 +1783,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="30" customHeight="1">
       <c r="A78" s="1">
         <v>6</v>
       </c>
@@ -1782,7 +1797,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="30" customHeight="1">
       <c r="A79" s="1">
         <v>6</v>
       </c>
@@ -1884,4 +1899,1443 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId79"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30">
+      <c r="A2" s="7">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9">
+        <v>8.9</v>
+      </c>
+      <c r="E2" s="7">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60">
+      <c r="A3" s="7">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E3" s="7">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E4" s="7">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="9">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E5" s="7">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E7" s="7">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E8" s="7">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="75">
+      <c r="A9" s="7">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E9" s="7">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="7">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E10" s="7">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="7">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E11" s="7">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45">
+      <c r="A12" s="7">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E12" s="7">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="7">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E13" s="7">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45">
+      <c r="A14" s="7">
+        <v>5</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E14" s="7">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45">
+      <c r="A15" s="7">
+        <v>5</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E15" s="7">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="7">
+        <v>5</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E16" s="7">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30">
+      <c r="A17" s="7">
+        <v>4</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E17" s="7">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60">
+      <c r="A18" s="7">
+        <v>3</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="7">
+        <v>5</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E19" s="7">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" s="7">
+        <v>5</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E20" s="7">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="7">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E21" s="7">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60">
+      <c r="A22" s="7">
+        <v>2</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E22" s="7">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45">
+      <c r="A23" s="7">
+        <v>6</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E23" s="7">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45">
+      <c r="A24" s="7">
+        <v>2</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E24" s="7">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45">
+      <c r="A25" s="7">
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E25" s="7">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="7">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E26" s="7">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="90">
+      <c r="A27" s="7">
+        <v>3</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="E27" s="7">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="7">
+        <v>5</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="E28" s="7">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="7">
+        <v>6</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="E29" s="7">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60">
+      <c r="A30" s="7">
+        <v>3</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="E30" s="7">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45">
+      <c r="A31" s="7">
+        <v>5</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="E31" s="7">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45">
+      <c r="A32" s="7">
+        <v>3</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="E32" s="7">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30">
+      <c r="A33" s="7">
+        <v>2</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="E33" s="7">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45">
+      <c r="A34" s="7">
+        <v>2</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="E34" s="7">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45">
+      <c r="A35" s="7">
+        <v>5</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E35" s="7">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30">
+      <c r="A36" s="7">
+        <v>4</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E36" s="7">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30">
+      <c r="A37" s="7">
+        <v>4</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E37" s="7">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="60">
+      <c r="A38" s="7">
+        <v>2</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E38" s="7">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45">
+      <c r="A39" s="7">
+        <v>3</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E39" s="7">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30">
+      <c r="A40" s="7">
+        <v>4</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E40" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="45">
+      <c r="A41" s="7">
+        <v>6</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E41" s="7">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30">
+      <c r="A42" s="7">
+        <v>2</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E42" s="7">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="45">
+      <c r="A43" s="7">
+        <v>1</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E43" s="7">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" s="7">
+        <v>4</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E44" s="7">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30">
+      <c r="A45" s="7">
+        <v>6</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E45" s="7">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="7">
+        <v>1</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E46" s="7">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="60">
+      <c r="A47" s="7">
+        <v>4</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E47" s="7">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30">
+      <c r="A48" s="7">
+        <v>2</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E48" s="7">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" s="7">
+        <v>5</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E49" s="7">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="45">
+      <c r="A50" s="7">
+        <v>1</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E50" s="7">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30">
+      <c r="A51" s="7">
+        <v>3</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E51" s="7">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="45">
+      <c r="A52" s="7">
+        <v>3</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E52" s="7">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="45">
+      <c r="A53" s="7">
+        <v>3</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E53" s="7">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30">
+      <c r="A54" s="7">
+        <v>5</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E54" s="7">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="45">
+      <c r="A55" s="7">
+        <v>6</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E55" s="7">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="45">
+      <c r="A56" s="7">
+        <v>3</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E56" s="7">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30">
+      <c r="A57" s="7">
+        <v>5</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E57" s="7">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="45">
+      <c r="A58" s="7">
+        <v>6</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="9">
+        <v>8.1</v>
+      </c>
+      <c r="E58" s="7">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30">
+      <c r="A59" s="7">
+        <v>1</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="9">
+        <v>8.1</v>
+      </c>
+      <c r="E59" s="7">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="7">
+        <v>6</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="9">
+        <v>8.1</v>
+      </c>
+      <c r="E60" s="7">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="7">
+        <v>3</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="9">
+        <v>8.1</v>
+      </c>
+      <c r="E61" s="7">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="7">
+        <v>1</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" s="9">
+        <v>8</v>
+      </c>
+      <c r="E62" s="7">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="7">
+        <v>3</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="9">
+        <v>8</v>
+      </c>
+      <c r="E63" s="7">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="45">
+      <c r="A64" s="7">
+        <v>2</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" s="9">
+        <v>8</v>
+      </c>
+      <c r="E64" s="7">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30">
+      <c r="A65" s="7">
+        <v>2</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D65" s="9">
+        <v>8</v>
+      </c>
+      <c r="E65" s="7">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30">
+      <c r="A66" s="7">
+        <v>2</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" s="9">
+        <v>8</v>
+      </c>
+      <c r="E66" s="7">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30">
+      <c r="A67" s="7">
+        <v>1</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="9">
+        <v>8</v>
+      </c>
+      <c r="E67" s="7">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="60">
+      <c r="A68" s="7">
+        <v>3</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="E68" s="7">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="60">
+      <c r="A69" s="7">
+        <v>1</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="E69" s="10">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45">
+      <c r="A70" s="7">
+        <v>2</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="E70" s="7">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="7">
+        <v>2</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="E71" s="7">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30">
+      <c r="A72" s="7">
+        <v>5</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D72" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="E72" s="7">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="45">
+      <c r="A73" s="7">
+        <v>6</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D73" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="E73" s="7">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="7">
+        <v>1</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D74" s="9">
+        <v>7.8</v>
+      </c>
+      <c r="E74" s="7">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="45">
+      <c r="A75" s="7">
+        <v>1</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D75" s="9">
+        <v>7.8</v>
+      </c>
+      <c r="E75" s="7">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="75">
+      <c r="A76" s="7">
+        <v>2</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D76" s="9">
+        <v>7.8</v>
+      </c>
+      <c r="E76" s="7">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45">
+      <c r="A77" s="7">
+        <v>6</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="9">
+        <v>7.7</v>
+      </c>
+      <c r="E77" s="7">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30">
+      <c r="A78" s="7">
+        <v>1</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D78" s="9">
+        <v>7.7</v>
+      </c>
+      <c r="E78" s="7">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30">
+      <c r="A79" s="7">
+        <v>1</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D79" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="E79" s="7">
+        <v>832</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="http://www.imdb.com/title/tt2939968/"/>
+    <hyperlink ref="C3" r:id="rId2" display="http://www.imdb.com/title/tt2717850/"/>
+    <hyperlink ref="C4" r:id="rId3" display="http://www.imdb.com/title/tt1102103/"/>
+    <hyperlink ref="C5" r:id="rId4" display="http://www.imdb.com/title/tt1484251/"/>
+    <hyperlink ref="C6" r:id="rId5" display="http://www.imdb.com/title/tt1615666/"/>
+    <hyperlink ref="C7" r:id="rId6" display="http://www.imdb.com/title/tt1615657/"/>
+    <hyperlink ref="C8" r:id="rId7" display="http://www.imdb.com/title/tt1615668/"/>
+    <hyperlink ref="C9" r:id="rId8" display="http://www.imdb.com/title/tt1615664/"/>
+    <hyperlink ref="C10" r:id="rId9" display="http://www.imdb.com/title/tt2939964/"/>
+    <hyperlink ref="C11" r:id="rId10" display="http://www.imdb.com/title/tt2939970/"/>
+    <hyperlink ref="C12" r:id="rId11" display="http://www.imdb.com/title/tt1615656/"/>
+    <hyperlink ref="C13" r:id="rId12" display="http://www.imdb.com/title/tt1615662/"/>
+    <hyperlink ref="C14" r:id="rId13" display="http://www.imdb.com/title/tt2049173/"/>
+    <hyperlink ref="C15" r:id="rId14" display="http://www.imdb.com/title/tt2049168/"/>
+    <hyperlink ref="C16" r:id="rId15" display="http://www.imdb.com/title/tt2049171/"/>
+    <hyperlink ref="C17" r:id="rId16" display="http://www.imdb.com/title/tt1615665/"/>
+    <hyperlink ref="C18" r:id="rId17" display="http://www.imdb.com/title/tt1484414/"/>
+    <hyperlink ref="C19" r:id="rId18" display="http://www.imdb.com/title/tt2049172/"/>
+    <hyperlink ref="C20" r:id="rId19" display="http://www.imdb.com/title/tt2048448/"/>
+    <hyperlink ref="C21" r:id="rId20" display="http://www.imdb.com/title/tt1105057/"/>
+    <hyperlink ref="C22" r:id="rId21" display="http://www.imdb.com/title/tt1118055/"/>
+    <hyperlink ref="C23" r:id="rId22" display="http://www.imdb.com/title/tt2882248/"/>
+    <hyperlink ref="C24" r:id="rId23" display="http://www.imdb.com/title/tt1118054/"/>
+    <hyperlink ref="C25" r:id="rId24" display="http://www.imdb.com/title/tt1615667/"/>
+    <hyperlink ref="C26" r:id="rId25" display="http://www.imdb.com/title/tt2049170/"/>
+    <hyperlink ref="C27" r:id="rId26" display="http://www.imdb.com/title/tt1484435/"/>
+    <hyperlink ref="C28" r:id="rId27" display="http://www.imdb.com/title/tt2049167/"/>
+    <hyperlink ref="C29" r:id="rId28" display="http://www.imdb.com/title/tt2882250/"/>
+    <hyperlink ref="C30" r:id="rId29" display="http://www.imdb.com/title/tt1484250/"/>
+    <hyperlink ref="C31" r:id="rId30" display="http://www.imdb.com/title/tt2049165/"/>
+    <hyperlink ref="C32" r:id="rId31" display="http://www.imdb.com/title/tt1472778/"/>
+    <hyperlink ref="C33" r:id="rId32" display="http://www.imdb.com/title/tt1118061/"/>
+    <hyperlink ref="C34" r:id="rId33" display="http://www.imdb.com/title/tt1118063/"/>
+    <hyperlink ref="C35" r:id="rId34" display="http://www.imdb.com/title/tt2049166/"/>
+    <hyperlink ref="C36" r:id="rId35" display="http://www.imdb.com/title/tt1615658/"/>
+    <hyperlink ref="C37" r:id="rId36" display="http://www.imdb.com/title/tt1615663/"/>
+    <hyperlink ref="C38" r:id="rId37" display="http://www.imdb.com/title/tt1118062/"/>
+    <hyperlink ref="C39" r:id="rId38" display="http://www.imdb.com/title/tt1484249/"/>
+    <hyperlink ref="C40" r:id="rId39" display="http://www.imdb.com/title/tt1615659/"/>
+    <hyperlink ref="C41" r:id="rId40" display="http://www.imdb.com/title/tt2560864/"/>
+    <hyperlink ref="C42" r:id="rId41" display="http://www.imdb.com/title/tt1118059/"/>
+    <hyperlink ref="C43" r:id="rId42" display="http://www.imdb.com/title/tt1097128/"/>
+    <hyperlink ref="C44" r:id="rId43" display="http://www.imdb.com/title/tt1615660/"/>
+    <hyperlink ref="C45" r:id="rId44" display="http://www.imdb.com/title/tt2717848/"/>
+    <hyperlink ref="C46" r:id="rId45" display="http://www.imdb.com/title/tt1097298/"/>
+    <hyperlink ref="C47" r:id="rId46" display="http://www.imdb.com/title/tt1615661/"/>
+    <hyperlink ref="C48" r:id="rId47" display="http://www.imdb.com/title/tt1118053/"/>
+    <hyperlink ref="C49" r:id="rId48" display="http://www.imdb.com/title/tt2049164/"/>
+    <hyperlink ref="C50" r:id="rId49" display="http://www.imdb.com/title/tt1094472/"/>
+    <hyperlink ref="C51" r:id="rId50" display="http://www.imdb.com/title/tt1439792/"/>
+    <hyperlink ref="C52" r:id="rId51" display="http://www.imdb.com/title/tt1484415/"/>
+    <hyperlink ref="C53" r:id="rId52" display="http://www.imdb.com/title/tt1484416/"/>
+    <hyperlink ref="C54" r:id="rId53" display="http://www.imdb.com/title/tt2049174/"/>
+    <hyperlink ref="C55" r:id="rId54" display="http://www.imdb.com/title/tt2663614/"/>
+    <hyperlink ref="C56" r:id="rId55" display="http://www.imdb.com/title/tt1484663/"/>
+    <hyperlink ref="C57" r:id="rId56" display="http://www.imdb.com/title/tt2049175/"/>
+    <hyperlink ref="C58" r:id="rId57" display="http://www.imdb.com/title/tt2939966/"/>
+    <hyperlink ref="C59" r:id="rId58" display="http://www.imdb.com/title/tt1108366/"/>
+    <hyperlink ref="C60" r:id="rId59" display="http://www.imdb.com/title/tt2551222/"/>
+    <hyperlink ref="C61" r:id="rId60" display="http://www.imdb.com/title/tt1484662/"/>
+    <hyperlink ref="C62" r:id="rId61" display="http://www.imdb.com/title/tt1097127/"/>
+    <hyperlink ref="C63" r:id="rId62" display="http://www.imdb.com/title/tt1484417/"/>
+    <hyperlink ref="C64" r:id="rId63" display="http://www.imdb.com/title/tt1118052/"/>
+    <hyperlink ref="C65" r:id="rId64" display="http://www.imdb.com/title/tt1118058/"/>
+    <hyperlink ref="C66" r:id="rId65" display="http://www.imdb.com/title/tt1118060/"/>
+    <hyperlink ref="C67" r:id="rId66" display="http://www.imdb.com/title/tt1050979/"/>
+    <hyperlink ref="C68" r:id="rId67" display="http://www.imdb.com/title/tt1449612/"/>
+    <hyperlink ref="C69" r:id="rId68" display="http://www.imdb.com/title/tt1059578/"/>
+    <hyperlink ref="C70" r:id="rId69" display="http://www.imdb.com/title/tt1118057/"/>
+    <hyperlink ref="C71" r:id="rId70" display="http://www.imdb.com/title/tt1118056/"/>
+    <hyperlink ref="C72" r:id="rId71" display="http://www.imdb.com/title/tt2049169/"/>
+    <hyperlink ref="C73" r:id="rId72" display="http://www.imdb.com/title/tt2649564/"/>
+    <hyperlink ref="C74" r:id="rId73" display="http://www.imdb.com/title/tt1042049/"/>
+    <hyperlink ref="C75" r:id="rId74" display="http://www.imdb.com/title/tt1040713/"/>
+    <hyperlink ref="C76" r:id="rId75" display="http://www.imdb.com/title/tt1118051/"/>
+    <hyperlink ref="C77" r:id="rId76" display="http://www.imdb.com/title/tt2470504/"/>
+    <hyperlink ref="C78" r:id="rId77" display="http://www.imdb.com/title/tt1049716/"/>
+    <hyperlink ref="C79" r:id="rId78" display="http://www.imdb.com/title/tt1049715/"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId79"/>
+</worksheet>
 </file>
</xml_diff>